<commit_message>
Debug : TXIQ_CDC & Change : DAC_DISABLE
</commit_message>
<xml_diff>
--- a/maia-hdl/projects/pluto/Table.xlsx
+++ b/maia-hdl/projects/pluto/Table.xlsx
@@ -23,19 +23,19 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Path 191</t>
+    <t>Path 209</t>
   </si>
   <si>
     <t>Slack</t>
   </si>
   <si>
-    <t>-5.117ns</t>
+    <t>-5.624ns</t>
   </si>
   <si>
     <t>Source</t>
   </si>
   <si>
-    <t>i_system_wrapper/system_i/maia_sdr/inst/control_registers/control/field_sdr_reset_reg/C   (rising edge-triggered cell FDSE clocked by clk_fpga_0  {rise@0.000ns fall@5.000ns period=10.000ns})</t>
+    <t>i_system_wrapper/system_i/maia_sdr/inst/txiq_cdc/sync_reset_w/stage1_reg/C   (rising edge-triggered cell FDRE clocked by clk_out1_system_maia_sdr_clk_0  {rise@0.000ns fall@8.000ns period=16.000ns})</t>
   </si>
   <si>
     <t>Destination</t>
@@ -59,13 +59,13 @@
     <t>Requirement</t>
   </si>
   <si>
-    <t>0.011ns (rx_clk rise@9160.011ns - clk_fpga_0 rise@9160.000ns)</t>
+    <t>0.031ns (rx_clk rise@14464.030ns - clk_out1_system_maia_sdr_clk_0 rise@14464.000ns)</t>
   </si>
   <si>
     <t>Data Path Delay</t>
   </si>
   <si>
-    <t>3.958ns (logic 0.456ns (11.521%)  route 3.502ns (88.479%))</t>
+    <t>0.838ns (logic 0.456ns (54.437%)  route 0.382ns (45.563%))</t>
   </si>
   <si>
     <t>Logic Levels</t>
@@ -77,13 +77,13 @@
     <t>Clock Path Skew</t>
   </si>
   <si>
-    <t>1.352ns</t>
+    <t>-2.274ns</t>
   </si>
   <si>
     <t>Clock Uncertainty</t>
   </si>
   <si>
-    <t>0.154ns</t>
+    <t>0.175ns</t>
   </si>
   <si>
     <t>Clock Domain Crossing</t>
@@ -158,7 +158,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="23.59375" customWidth="true"/>
-    <col min="2" max="2" width="195.0" customWidth="true"/>
+    <col min="2" max="2" width="206.09375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>